<commit_message>
new text files for new taggings :)
</commit_message>
<xml_diff>
--- a/training/data/tagging.xlsx
+++ b/training/data/tagging.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4167e8f1ae5040c7/Documents/political-campaign-project/training/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4167e8f1ae5040c7/Documents/GitHub/political-campaign-project/training/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="39" documentId="8_{F413C203-8A3D-499D-A834-4C2CD2B203CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EFACF573-C225-47A0-9970-AF1AD5384205}"/>
+  <xr:revisionPtr revIDLastSave="40" documentId="8_{F413C203-8A3D-499D-A834-4C2CD2B203CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7CD58B87-529F-4008-975D-A0ADD9666E40}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tagging" sheetId="1" r:id="rId1"/>
@@ -1710,19 +1710,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:O188"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="A155" workbookViewId="0">
+      <selection activeCell="E170" sqref="E170"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="61" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1757,7 +1756,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="2" spans="1:15" hidden="1" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1790,7 +1789,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -1823,7 +1822,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -1862,7 +1861,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -1892,7 +1891,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -1922,7 +1921,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -1952,7 +1951,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -1985,7 +1984,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -2018,7 +2017,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -2051,7 +2050,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -2084,7 +2083,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -2117,7 +2116,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:15" hidden="1" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -2150,7 +2149,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -2183,7 +2182,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -2216,7 +2215,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -2249,7 +2248,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="17" spans="1:15" hidden="1" x14ac:dyDescent="0.75">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>25</v>
       </c>
@@ -2285,7 +2284,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>26</v>
       </c>
@@ -2318,7 +2317,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -2354,7 +2353,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>28</v>
       </c>
@@ -2381,7 +2380,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>29</v>
       </c>
@@ -2414,7 +2413,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>30</v>
       </c>
@@ -2450,7 +2449,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="23" spans="1:15" hidden="1" x14ac:dyDescent="0.75">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>31</v>
       </c>
@@ -2483,7 +2482,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="24" spans="1:15" hidden="1" x14ac:dyDescent="0.75">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>32</v>
       </c>
@@ -2516,7 +2515,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="25" spans="1:15" hidden="1" x14ac:dyDescent="0.75">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>33</v>
       </c>
@@ -2549,7 +2548,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="26" spans="1:15" hidden="1" x14ac:dyDescent="0.75">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>35</v>
       </c>
@@ -2582,7 +2581,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>36</v>
       </c>
@@ -2615,7 +2614,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="28" spans="1:15" hidden="1" x14ac:dyDescent="0.75">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>37</v>
       </c>
@@ -2648,7 +2647,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>38</v>
       </c>
@@ -2681,7 +2680,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="30" spans="1:15" hidden="1" x14ac:dyDescent="0.75">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>39</v>
       </c>
@@ -2714,7 +2713,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>40</v>
       </c>
@@ -2747,7 +2746,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>41</v>
       </c>
@@ -2780,7 +2779,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>42</v>
       </c>
@@ -2810,7 +2809,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>43</v>
       </c>
@@ -2843,7 +2842,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="35" spans="1:15" hidden="1" x14ac:dyDescent="0.75">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>44</v>
       </c>
@@ -2876,7 +2875,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="36" spans="1:15" hidden="1" x14ac:dyDescent="0.75">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>45</v>
       </c>
@@ -2912,7 +2911,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>46</v>
       </c>
@@ -2945,7 +2944,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="38" spans="1:15" hidden="1" x14ac:dyDescent="0.75">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>47</v>
       </c>
@@ -2978,7 +2977,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>48</v>
       </c>
@@ -3011,7 +3010,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>49</v>
       </c>
@@ -3044,7 +3043,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>50</v>
       </c>
@@ -3080,7 +3079,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>51</v>
       </c>
@@ -3113,7 +3112,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="43" spans="1:15" hidden="1" x14ac:dyDescent="0.75">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>52</v>
       </c>
@@ -3146,7 +3145,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>53</v>
       </c>
@@ -3179,7 +3178,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>54</v>
       </c>
@@ -3212,7 +3211,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="46" spans="1:15" hidden="1" x14ac:dyDescent="0.75">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>55</v>
       </c>
@@ -3245,7 +3244,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>56</v>
       </c>
@@ -3278,7 +3277,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="48" spans="1:15" hidden="1" x14ac:dyDescent="0.75">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>57</v>
       </c>
@@ -3317,7 +3316,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>58</v>
       </c>
@@ -3350,7 +3349,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>59</v>
       </c>
@@ -3380,7 +3379,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>60</v>
       </c>
@@ -3413,7 +3412,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>61</v>
       </c>
@@ -3440,7 +3439,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="53" spans="1:15" hidden="1" x14ac:dyDescent="0.75">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>62</v>
       </c>
@@ -3473,7 +3472,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>63</v>
       </c>
@@ -3506,7 +3505,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="55" spans="1:15" hidden="1" x14ac:dyDescent="0.75">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>64</v>
       </c>
@@ -3539,7 +3538,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="56" spans="1:15" hidden="1" x14ac:dyDescent="0.75">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>65</v>
       </c>
@@ -3572,7 +3571,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>66</v>
       </c>
@@ -3605,7 +3604,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="58" spans="1:15" hidden="1" x14ac:dyDescent="0.75">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>67</v>
       </c>
@@ -3641,7 +3640,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>68</v>
       </c>
@@ -3674,7 +3673,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>69</v>
       </c>
@@ -3707,7 +3706,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>70</v>
       </c>
@@ -3737,7 +3736,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>71</v>
       </c>
@@ -3770,7 +3769,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>72</v>
       </c>
@@ -3803,7 +3802,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>73</v>
       </c>
@@ -3833,7 +3832,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="65" spans="1:15" hidden="1" x14ac:dyDescent="0.75">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>75</v>
       </c>
@@ -3866,7 +3865,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>76</v>
       </c>
@@ -3899,7 +3898,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>77</v>
       </c>
@@ -3932,7 +3931,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>78</v>
       </c>
@@ -3962,7 +3961,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>79</v>
       </c>
@@ -3995,7 +3994,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="70" spans="1:15" hidden="1" x14ac:dyDescent="0.75">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>80</v>
       </c>
@@ -4028,7 +4027,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>81</v>
       </c>
@@ -4061,7 +4060,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>82</v>
       </c>
@@ -4094,7 +4093,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>83</v>
       </c>
@@ -4127,7 +4126,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="74" spans="1:15" hidden="1" x14ac:dyDescent="0.75">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>84</v>
       </c>
@@ -4160,7 +4159,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>85</v>
       </c>
@@ -4190,7 +4189,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="76" spans="1:15" hidden="1" x14ac:dyDescent="0.75">
+    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>86</v>
       </c>
@@ -4223,7 +4222,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>87</v>
       </c>
@@ -4259,7 +4258,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>88</v>
       </c>
@@ -4292,7 +4291,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>89</v>
       </c>
@@ -4325,7 +4324,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>90</v>
       </c>
@@ -4361,7 +4360,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="81" spans="1:15" hidden="1" x14ac:dyDescent="0.75">
+    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>91</v>
       </c>
@@ -4391,7 +4390,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="82" spans="1:15" hidden="1" x14ac:dyDescent="0.75">
+    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>92</v>
       </c>
@@ -4424,7 +4423,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="83" spans="1:15" hidden="1" x14ac:dyDescent="0.75">
+    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>93</v>
       </c>
@@ -4460,7 +4459,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="84" spans="1:15" hidden="1" x14ac:dyDescent="0.75">
+    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>94</v>
       </c>
@@ -4493,7 +4492,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>95</v>
       </c>
@@ -4523,7 +4522,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>96</v>
       </c>
@@ -4553,7 +4552,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>97</v>
       </c>
@@ -4580,7 +4579,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>98</v>
       </c>
@@ -4610,7 +4609,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:15" hidden="1" x14ac:dyDescent="0.75">
+    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>99</v>
       </c>
@@ -4643,7 +4642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:15" hidden="1" x14ac:dyDescent="0.75">
+    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>100</v>
       </c>
@@ -4670,7 +4669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>101</v>
       </c>
@@ -4700,7 +4699,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>102</v>
       </c>
@@ -4730,7 +4729,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:15" hidden="1" x14ac:dyDescent="0.75">
+    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>103</v>
       </c>
@@ -4760,7 +4759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:15" hidden="1" x14ac:dyDescent="0.75">
+    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>104</v>
       </c>
@@ -4793,7 +4792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.75">
+    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>105</v>
       </c>
@@ -4823,7 +4822,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:15" hidden="1" x14ac:dyDescent="0.75">
+    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>106</v>
       </c>
@@ -4853,7 +4852,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>107</v>
       </c>
@@ -4883,7 +4882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>108</v>
       </c>
@@ -4907,7 +4906,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>109</v>
       </c>
@@ -4934,7 +4933,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>110</v>
       </c>
@@ -4964,7 +4963,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>111</v>
       </c>
@@ -4994,7 +4993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>112</v>
       </c>
@@ -5024,7 +5023,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>113</v>
       </c>
@@ -5054,7 +5053,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>114</v>
       </c>
@@ -5090,7 +5089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>115</v>
       </c>
@@ -5120,7 +5119,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>116</v>
       </c>
@@ -5144,7 +5143,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>117</v>
       </c>
@@ -5174,7 +5173,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>118</v>
       </c>
@@ -5204,7 +5203,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>119</v>
       </c>
@@ -5234,7 +5233,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>120</v>
       </c>
@@ -5264,7 +5263,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>121</v>
       </c>
@@ -5294,7 +5293,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>122</v>
       </c>
@@ -5324,7 +5323,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>123</v>
       </c>
@@ -5354,7 +5353,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>124</v>
       </c>
@@ -5384,7 +5383,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>125</v>
       </c>
@@ -5414,7 +5413,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>126</v>
       </c>
@@ -5444,7 +5443,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>127</v>
       </c>
@@ -5474,7 +5473,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>128</v>
       </c>
@@ -5504,7 +5503,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>129</v>
       </c>
@@ -5534,7 +5533,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>130</v>
       </c>
@@ -5561,7 +5560,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>131</v>
       </c>
@@ -5591,7 +5590,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>132</v>
       </c>
@@ -5618,7 +5617,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>133</v>
       </c>
@@ -5651,7 +5650,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>134</v>
       </c>
@@ -5681,7 +5680,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>135</v>
       </c>
@@ -5711,7 +5710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>136</v>
       </c>
@@ -5744,7 +5743,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>137</v>
       </c>
@@ -5774,7 +5773,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>138</v>
       </c>
@@ -5804,7 +5803,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>139</v>
       </c>
@@ -5831,7 +5830,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>140</v>
       </c>
@@ -5861,7 +5860,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>141</v>
       </c>
@@ -5891,7 +5890,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>142</v>
       </c>
@@ -5915,7 +5914,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>143</v>
       </c>
@@ -5945,7 +5944,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>144</v>
       </c>
@@ -5975,7 +5974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>145</v>
       </c>
@@ -6011,7 +6010,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>146</v>
       </c>
@@ -6041,7 +6040,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>147</v>
       </c>
@@ -6071,7 +6070,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>148</v>
       </c>
@@ -6098,7 +6097,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>149</v>
       </c>
@@ -6128,7 +6127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>150</v>
       </c>
@@ -6158,7 +6157,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>151</v>
       </c>
@@ -6188,7 +6187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>152</v>
       </c>
@@ -6212,7 +6211,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>153</v>
       </c>
@@ -6245,7 +6244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>154</v>
       </c>
@@ -6275,7 +6274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>155</v>
       </c>
@@ -6305,7 +6304,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>156</v>
       </c>
@@ -6335,7 +6334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>157</v>
       </c>
@@ -6368,7 +6367,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>158</v>
       </c>
@@ -6404,7 +6403,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>159</v>
       </c>
@@ -6434,7 +6433,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>160</v>
       </c>
@@ -6467,7 +6466,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>161</v>
       </c>
@@ -6497,7 +6496,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>162</v>
       </c>
@@ -6530,7 +6529,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>163</v>
       </c>
@@ -6554,7 +6553,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>164</v>
       </c>
@@ -6584,7 +6583,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>165</v>
       </c>
@@ -6614,7 +6613,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>166</v>
       </c>
@@ -6647,7 +6646,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>167</v>
       </c>
@@ -6677,7 +6676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>168</v>
       </c>
@@ -6710,7 +6709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>169</v>
       </c>
@@ -6743,7 +6742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>170</v>
       </c>
@@ -6773,7 +6772,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>171</v>
       </c>
@@ -6806,7 +6805,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>172</v>
       </c>
@@ -6836,7 +6835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>173</v>
       </c>
@@ -6866,7 +6865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>174</v>
       </c>
@@ -6890,7 +6889,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>175</v>
       </c>
@@ -6917,7 +6916,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>176</v>
       </c>
@@ -6941,7 +6940,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>177</v>
       </c>
@@ -6971,7 +6970,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="168" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>178</v>
       </c>
@@ -6998,7 +6997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>179</v>
       </c>
@@ -7028,7 +7027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>180</v>
       </c>
@@ -7052,7 +7051,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>181</v>
       </c>
@@ -7082,7 +7081,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>182</v>
       </c>
@@ -7112,7 +7111,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="173" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+    <row r="173" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>183</v>
       </c>
@@ -7142,7 +7141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="174" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>184</v>
       </c>
@@ -7169,7 +7168,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="175" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+    <row r="175" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>185</v>
       </c>
@@ -7202,7 +7201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="176" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>186</v>
       </c>
@@ -7235,7 +7234,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="177" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="177" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>187</v>
       </c>
@@ -7268,7 +7267,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="178" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+    <row r="178" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>188</v>
       </c>
@@ -7298,7 +7297,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+    <row r="179" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>189</v>
       </c>
@@ -7331,7 +7330,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="180" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>190</v>
       </c>
@@ -7361,7 +7360,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="181" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="181" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>191</v>
       </c>
@@ -7391,7 +7390,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="182" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="182" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>192</v>
       </c>
@@ -7418,7 +7417,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="183" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="183" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>193</v>
       </c>
@@ -7445,7 +7444,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="184" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="184" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>194</v>
       </c>
@@ -7475,7 +7474,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="185" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="185" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>195</v>
       </c>
@@ -7508,7 +7507,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="186" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+    <row r="186" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>196</v>
       </c>
@@ -7538,7 +7537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:11" hidden="1" x14ac:dyDescent="0.75">
+    <row r="187" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>197</v>
       </c>
@@ -7568,7 +7567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="188" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>198</v>
       </c>
@@ -7599,13 +7598,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K188" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="10">
-      <filters>
-        <filter val="TRUE"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>